<commit_message>
Atualização automática de MONTENEGRO.xlsx
</commit_message>
<xml_diff>
--- a/MONTENEGRO.xlsx
+++ b/MONTENEGRO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41DC771E-8E7F-4B16-ACAC-1DFEAB4FC9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4212FE4-F747-4920-AFD3-4A9C5B039856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,20 +21,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="5" r:id="rId6"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1083,7 +1070,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1143,36 +1130,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1211,14 +1174,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1264,7 +1222,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{CF52B63F-7913-418D-80CC-129DEE17B9CC}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{3A827CF0-B243-4B4B-9304-DB22AFB999B8}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1294,10 +1252,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75D5C290-33C1-45AA-8D2E-E1D0D5148047}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECCBC65B-8303-4669-9F81-2DA5D848F63A}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1335,7 +1293,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A16D682-F081-4DE2-BFE3-30BB18F46796}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4489746-04A8-4871-8D5D-0476C1F0B4AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1398,7 +1356,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BBCCF8D-B005-4D5E-9B1B-202A9AE1B1CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F14C75B-F8FC-48D5-8730-84E8483578CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1417,7 +1375,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0751DE3-0007-6475-8FC7-3FE560E5E0F9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCAFF935-1FD8-CFC3-9D44-D0415111DD17}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1466,7 +1424,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C06865AA-4B91-66B7-B5CE-92016C0A0B27}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5217AD7-2504-73C1-2266-603740FA8B44}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1485,7 +1443,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D3D6374-04D7-DAFC-8E5F-A3A7742219A3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9747711-8623-B8B6-B173-2BFE313A12DB}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1516,7 +1474,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA88E3AD-9CBD-1312-E5E9-6E446A114F5D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{801899E0-A64D-8C01-796F-BCFE689476B4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1547,7 +1505,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E62F659E-E430-CB4A-7FD2-26CFD1ABE3A4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB47D06B-3EBE-CBF1-4406-842B6478A9FA}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1590,7 +1548,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3937D45-D6B6-45E5-972E-124B29582643}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D3AF8AD-70D2-4265-AC82-61F10E972C39}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1628,7 +1586,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DF3350B-B59D-467B-BBA4-D16DA3658F48}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37B4714F-4A68-4537-B263-477F698AFC90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1671,7 +1629,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1FAA031-439E-41A3-8443-E033550CF29F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{137DB5D4-FF98-4C1B-98BD-D525630BF30D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1984,7 +1942,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87B44EE9-82AD-4857-8729-96FD690E8E08}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C637F988-0F98-45A1-8400-0EB378D4DB73}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1996,98 +1954,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="37"/>
-    <col min="6" max="6" width="2" style="37" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="37" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="37"/>
+    <col min="1" max="5" width="12.5703125" style="34"/>
+    <col min="6" max="6" width="2" style="34" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="34" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="36"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="36"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="36"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="36"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="36"/>
+      <c r="F5" s="33"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="36"/>
+      <c r="F6" s="33"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="36"/>
+      <c r="F7" s="33"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="36"/>
+      <c r="F8" s="33"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="36"/>
+      <c r="F9" s="33"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="36"/>
+      <c r="F10" s="33"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="36"/>
+      <c r="F11" s="33"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="36"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="36"/>
+      <c r="F13" s="33"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="36"/>
+      <c r="F14" s="33"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="36"/>
+      <c r="F15" s="33"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="36"/>
+      <c r="F16" s="33"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="36"/>
+      <c r="F17" s="33"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="36"/>
+      <c r="F18" s="33"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="36"/>
+      <c r="F19" s="33"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="36"/>
+      <c r="F20" s="33"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="36"/>
+      <c r="F21" s="33"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="36"/>
+      <c r="F22" s="33"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="36"/>
+      <c r="F23" s="33"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="36"/>
+      <c r="F24" s="33"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="36"/>
+      <c r="F25" s="33"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="36"/>
+      <c r="F26" s="33"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="36"/>
+      <c r="F27" s="33"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="36"/>
+      <c r="F28" s="33"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="36"/>
+      <c r="F29" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5355,19 +5313,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>273</v>
       </c>
     </row>
@@ -5390,90 +5348,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="19" t="s">
         <v>280</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="19" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="19" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="19" t="s">
         <v>283</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="19" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="19" t="s">
         <v>277</v>
       </c>
     </row>
@@ -5498,54 +5456,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>285</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>286</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="22" t="s">
         <v>290</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="22" t="s">
         <v>291</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="20" t="s">
         <v>293</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="20" t="s">
         <v>294</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="20" t="s">
         <v>295</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="20" t="s">
         <v>296</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="20" t="s">
         <v>297</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="20" t="s">
         <v>298</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="20" t="s">
         <v>299</v>
       </c>
     </row>
@@ -5556,41 +5515,41 @@
       <c r="B2" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="23">
         <v>45839</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="24" t="s">
         <v>301</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="25">
         <v>22899</v>
       </c>
-      <c r="G2" s="28">
+      <c r="G2" s="25">
         <v>2845</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="26" t="s">
         <v>303</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="26" t="s">
         <v>303</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="26" t="s">
         <v>303</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="26" t="s">
         <v>303</v>
       </c>
-      <c r="M2" s="30" t="s">
+      <c r="M2" s="27" t="s">
         <v>304</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="O2" s="30" t="s">
+      <c r="O2" s="27" t="s">
         <v>304</v>
       </c>
     </row>
@@ -5621,25 +5580,24 @@
       <c r="B1" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="28" t="s">
         <v>306</v>
       </c>
-      <c r="E1" s="32">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="29">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>307</v>
+      </c>
+      <c r="B2" s="32">
         <v>17</v>
       </c>
-      <c r="F1" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>307</v>
-      </c>
-      <c r="B2" s="35">
-        <v>17</v>
-      </c>
-      <c r="C2" s="33">
+      <c r="C2" s="30">
         <v>1.124189921967994E-3</v>
       </c>
     </row>

</xml_diff>